<commit_message>
corrected the topology man157
added the traffic data
</commit_message>
<xml_diff>
--- a/input_files/Metro_topology_MAN157.xlsx
+++ b/input_files/Metro_topology_MAN157.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otomy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otomy\Documents\GitHub\traffic-latency-simulator\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD19EF1-F55F-482F-B992-613680F117B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C38FE3A-69E3-4653-A960-E806E28ACECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
-    <sheet name="Links" sheetId="2" r:id="rId2"/>
-    <sheet name="EquipmentCost" sheetId="3" r:id="rId3"/>
-    <sheet name="EquipmentCost_v2" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Links" sheetId="2" r:id="rId3"/>
+    <sheet name="EquipmentCost" sheetId="3" r:id="rId4"/>
+    <sheet name="EquipmentCost_v2" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2439" uniqueCount="244">
   <si>
     <t>Node Type</t>
   </si>
@@ -759,6 +760,15 @@
   </si>
   <si>
     <t>node_code</t>
+  </si>
+  <si>
+    <t>trafficGbps</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>CWB</t>
   </si>
 </sst>
 </file>
@@ -769,10 +779,17 @@
     <numFmt numFmtId="164" formatCode="#,##0.000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -848,25 +865,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1203,11 +1221,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="5" max="5" width="24.08984375" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -7219,6 +7241,4524 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E25885F4-38A7-4535-955F-547BC97B198C}">
+  <dimension ref="A1:D345"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
+      <selection activeCell="G260" sqref="G260"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="16">
+        <v>0</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="16">
+        <v>0</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="16">
+        <v>0</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" s="16">
+        <v>0</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="16">
+        <v>0</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="16">
+        <v>0</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" s="16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" s="16">
+        <v>0</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" s="16">
+        <v>0</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" s="16">
+        <v>0</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" s="16">
+        <v>0</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" s="16">
+        <v>0</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" s="16">
+        <v>0</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" s="16">
+        <v>0</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" s="16">
+        <v>0</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" s="16">
+        <v>0</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" s="16">
+        <v>0</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" s="16">
+        <v>0</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" s="16">
+        <v>0</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" s="16">
+        <v>0</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" s="16">
+        <v>0</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" s="16">
+        <v>0</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34" s="16">
+        <v>0</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" s="16">
+        <v>0</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" s="16">
+        <v>0</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" s="16">
+        <v>0</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" s="16">
+        <v>0</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39" s="16">
+        <v>0</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40" s="16">
+        <v>0</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41">
+        <v>25</v>
+      </c>
+      <c r="C41" s="16">
+        <v>0</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42">
+        <v>25</v>
+      </c>
+      <c r="C42" s="16">
+        <v>0</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43">
+        <v>24</v>
+      </c>
+      <c r="C43" s="16">
+        <v>0</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44">
+        <v>25</v>
+      </c>
+      <c r="C44" s="16">
+        <v>0</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>126</v>
+      </c>
+      <c r="B45">
+        <v>24</v>
+      </c>
+      <c r="C45" s="16">
+        <v>0</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>127</v>
+      </c>
+      <c r="B46">
+        <v>24</v>
+      </c>
+      <c r="C46" s="16">
+        <v>0</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47">
+        <v>24</v>
+      </c>
+      <c r="C47" s="16">
+        <v>0</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48">
+        <v>24</v>
+      </c>
+      <c r="C48" s="16">
+        <v>0</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49">
+        <v>24</v>
+      </c>
+      <c r="C49" s="16">
+        <v>0</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50">
+        <v>24</v>
+      </c>
+      <c r="C50" s="16">
+        <v>0</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>132</v>
+      </c>
+      <c r="B51">
+        <v>25</v>
+      </c>
+      <c r="C51" s="16">
+        <v>0</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>133</v>
+      </c>
+      <c r="B52">
+        <v>25</v>
+      </c>
+      <c r="C52" s="16">
+        <v>0</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>134</v>
+      </c>
+      <c r="B53">
+        <v>24</v>
+      </c>
+      <c r="C53" s="16">
+        <v>0</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54">
+        <v>24</v>
+      </c>
+      <c r="C54" s="16">
+        <v>0</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55">
+        <v>25</v>
+      </c>
+      <c r="C55" s="16">
+        <v>0</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56">
+        <v>24</v>
+      </c>
+      <c r="C56" s="16">
+        <v>0</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57">
+        <v>24</v>
+      </c>
+      <c r="C57" s="16">
+        <v>0</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58">
+        <v>24</v>
+      </c>
+      <c r="C58" s="16">
+        <v>0</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59">
+        <v>10</v>
+      </c>
+      <c r="C59" s="16">
+        <v>0</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60">
+        <v>7</v>
+      </c>
+      <c r="C60" s="16">
+        <v>0</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61">
+        <v>7</v>
+      </c>
+      <c r="C61" s="16">
+        <v>0</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
+        <v>143</v>
+      </c>
+      <c r="B62">
+        <v>7</v>
+      </c>
+      <c r="C62" s="16">
+        <v>0</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>144</v>
+      </c>
+      <c r="B63">
+        <v>10</v>
+      </c>
+      <c r="C63" s="16">
+        <v>0</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>145</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+      <c r="C64" s="16">
+        <v>0</v>
+      </c>
+      <c r="D64" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>146</v>
+      </c>
+      <c r="B65">
+        <v>10</v>
+      </c>
+      <c r="C65" s="16">
+        <v>0</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>147</v>
+      </c>
+      <c r="B66">
+        <v>7</v>
+      </c>
+      <c r="C66" s="16">
+        <v>0</v>
+      </c>
+      <c r="D66" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>148</v>
+      </c>
+      <c r="B67">
+        <v>7</v>
+      </c>
+      <c r="C67" s="16">
+        <v>0</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>149</v>
+      </c>
+      <c r="B68">
+        <v>7</v>
+      </c>
+      <c r="C68" s="16">
+        <v>0</v>
+      </c>
+      <c r="D68" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>150</v>
+      </c>
+      <c r="B69">
+        <v>10</v>
+      </c>
+      <c r="C69" s="16">
+        <v>0</v>
+      </c>
+      <c r="D69" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>151</v>
+      </c>
+      <c r="B70">
+        <v>7</v>
+      </c>
+      <c r="C70" s="16">
+        <v>0</v>
+      </c>
+      <c r="D70" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>152</v>
+      </c>
+      <c r="B71">
+        <v>10</v>
+      </c>
+      <c r="C71" s="16">
+        <v>0</v>
+      </c>
+      <c r="D71" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>153</v>
+      </c>
+      <c r="B72">
+        <v>10</v>
+      </c>
+      <c r="C72" s="16">
+        <v>0</v>
+      </c>
+      <c r="D72" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>154</v>
+      </c>
+      <c r="B73">
+        <v>10</v>
+      </c>
+      <c r="C73" s="16">
+        <v>0</v>
+      </c>
+      <c r="D73" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>155</v>
+      </c>
+      <c r="B74">
+        <v>10</v>
+      </c>
+      <c r="C74" s="16">
+        <v>0</v>
+      </c>
+      <c r="D74" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>156</v>
+      </c>
+      <c r="B75">
+        <v>10</v>
+      </c>
+      <c r="C75" s="16">
+        <v>0</v>
+      </c>
+      <c r="D75" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76">
+        <v>10</v>
+      </c>
+      <c r="C76" s="16">
+        <v>0</v>
+      </c>
+      <c r="D76" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>158</v>
+      </c>
+      <c r="B77">
+        <v>37</v>
+      </c>
+      <c r="C77" s="16">
+        <v>0</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>159</v>
+      </c>
+      <c r="B78">
+        <v>37</v>
+      </c>
+      <c r="C78" s="16">
+        <v>0</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>160</v>
+      </c>
+      <c r="B79">
+        <v>37</v>
+      </c>
+      <c r="C79" s="16">
+        <v>0</v>
+      </c>
+      <c r="D79" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>161</v>
+      </c>
+      <c r="B80">
+        <v>37</v>
+      </c>
+      <c r="C80" s="16">
+        <v>0</v>
+      </c>
+      <c r="D80" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>162</v>
+      </c>
+      <c r="B81">
+        <v>37</v>
+      </c>
+      <c r="C81" s="16">
+        <v>0</v>
+      </c>
+      <c r="D81" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>163</v>
+      </c>
+      <c r="B82">
+        <v>37</v>
+      </c>
+      <c r="C82" s="16">
+        <v>0</v>
+      </c>
+      <c r="D82" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83">
+        <v>37</v>
+      </c>
+      <c r="C83" s="16">
+        <v>0</v>
+      </c>
+      <c r="D83" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84">
+        <v>37</v>
+      </c>
+      <c r="C84" s="16">
+        <v>0</v>
+      </c>
+      <c r="D84" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>166</v>
+      </c>
+      <c r="B85">
+        <v>37</v>
+      </c>
+      <c r="C85" s="16">
+        <v>0</v>
+      </c>
+      <c r="D85" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>167</v>
+      </c>
+      <c r="B86">
+        <v>37</v>
+      </c>
+      <c r="C86" s="16">
+        <v>0</v>
+      </c>
+      <c r="D86" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>168</v>
+      </c>
+      <c r="B87">
+        <v>37</v>
+      </c>
+      <c r="C87" s="16">
+        <v>0</v>
+      </c>
+      <c r="D87" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>169</v>
+      </c>
+      <c r="B88">
+        <v>39</v>
+      </c>
+      <c r="C88" s="16">
+        <v>0</v>
+      </c>
+      <c r="D88" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>170</v>
+      </c>
+      <c r="B89">
+        <v>37</v>
+      </c>
+      <c r="C89" s="16">
+        <v>0</v>
+      </c>
+      <c r="D89" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>171</v>
+      </c>
+      <c r="B90">
+        <v>39</v>
+      </c>
+      <c r="C90" s="16">
+        <v>0</v>
+      </c>
+      <c r="D90" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>172</v>
+      </c>
+      <c r="B91">
+        <v>39</v>
+      </c>
+      <c r="C91" s="16">
+        <v>0</v>
+      </c>
+      <c r="D91" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>173</v>
+      </c>
+      <c r="B92">
+        <v>39</v>
+      </c>
+      <c r="C92" s="16">
+        <v>0</v>
+      </c>
+      <c r="D92" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>174</v>
+      </c>
+      <c r="B93">
+        <v>39</v>
+      </c>
+      <c r="C93" s="16">
+        <v>0</v>
+      </c>
+      <c r="D93" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>175</v>
+      </c>
+      <c r="B94">
+        <v>37</v>
+      </c>
+      <c r="C94" s="16">
+        <v>0</v>
+      </c>
+      <c r="D94" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>176</v>
+      </c>
+      <c r="B95">
+        <v>19</v>
+      </c>
+      <c r="C95" s="16">
+        <v>0</v>
+      </c>
+      <c r="D95" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" t="s">
+        <v>177</v>
+      </c>
+      <c r="B96">
+        <v>24</v>
+      </c>
+      <c r="C96" s="16">
+        <v>0</v>
+      </c>
+      <c r="D96" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>178</v>
+      </c>
+      <c r="B97">
+        <v>15</v>
+      </c>
+      <c r="C97" s="16">
+        <v>0</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>179</v>
+      </c>
+      <c r="B98">
+        <v>24</v>
+      </c>
+      <c r="C98" s="16">
+        <v>0</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>180</v>
+      </c>
+      <c r="B99">
+        <v>15</v>
+      </c>
+      <c r="C99" s="16">
+        <v>0</v>
+      </c>
+      <c r="D99" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>181</v>
+      </c>
+      <c r="B100">
+        <v>19</v>
+      </c>
+      <c r="C100" s="16">
+        <v>0</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" t="s">
+        <v>182</v>
+      </c>
+      <c r="B101">
+        <v>15</v>
+      </c>
+      <c r="C101" s="16">
+        <v>0</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>183</v>
+      </c>
+      <c r="B102">
+        <v>15</v>
+      </c>
+      <c r="C102" s="16">
+        <v>0</v>
+      </c>
+      <c r="D102" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>184</v>
+      </c>
+      <c r="B103">
+        <v>19</v>
+      </c>
+      <c r="C103" s="16">
+        <v>0</v>
+      </c>
+      <c r="D103" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" t="s">
+        <v>185</v>
+      </c>
+      <c r="B104">
+        <v>15</v>
+      </c>
+      <c r="C104" s="16">
+        <v>0</v>
+      </c>
+      <c r="D104" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="s">
+        <v>186</v>
+      </c>
+      <c r="B105">
+        <v>16</v>
+      </c>
+      <c r="C105" s="16">
+        <v>0</v>
+      </c>
+      <c r="D105" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
+        <v>187</v>
+      </c>
+      <c r="B106">
+        <v>21</v>
+      </c>
+      <c r="C106" s="16">
+        <v>0</v>
+      </c>
+      <c r="D106" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>188</v>
+      </c>
+      <c r="B107">
+        <v>16</v>
+      </c>
+      <c r="C107" s="16">
+        <v>0</v>
+      </c>
+      <c r="D107" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>189</v>
+      </c>
+      <c r="B108">
+        <v>17</v>
+      </c>
+      <c r="C108" s="16">
+        <v>0</v>
+      </c>
+      <c r="D108" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="s">
+        <v>190</v>
+      </c>
+      <c r="B109">
+        <v>23</v>
+      </c>
+      <c r="C109" s="16">
+        <v>0</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>191</v>
+      </c>
+      <c r="B110">
+        <v>17</v>
+      </c>
+      <c r="C110" s="16">
+        <v>0</v>
+      </c>
+      <c r="D110" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>192</v>
+      </c>
+      <c r="B111">
+        <v>18</v>
+      </c>
+      <c r="C111" s="16">
+        <v>0</v>
+      </c>
+      <c r="D111" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>193</v>
+      </c>
+      <c r="B112">
+        <v>12</v>
+      </c>
+      <c r="C112" s="16">
+        <v>0</v>
+      </c>
+      <c r="D112" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>194</v>
+      </c>
+      <c r="B113">
+        <v>18</v>
+      </c>
+      <c r="C113" s="16">
+        <v>0</v>
+      </c>
+      <c r="D113" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>195</v>
+      </c>
+      <c r="B114">
+        <v>12</v>
+      </c>
+      <c r="C114" s="16">
+        <v>0</v>
+      </c>
+      <c r="D114" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>196</v>
+      </c>
+      <c r="B115">
+        <v>12</v>
+      </c>
+      <c r="C115" s="16">
+        <v>0</v>
+      </c>
+      <c r="D115" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>197</v>
+      </c>
+      <c r="B116">
+        <v>18</v>
+      </c>
+      <c r="C116" s="16">
+        <v>0</v>
+      </c>
+      <c r="D116" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>198</v>
+      </c>
+      <c r="B117">
+        <v>11</v>
+      </c>
+      <c r="C117" s="16">
+        <v>0</v>
+      </c>
+      <c r="D117" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>199</v>
+      </c>
+      <c r="B118">
+        <v>8</v>
+      </c>
+      <c r="C118" s="16">
+        <v>0</v>
+      </c>
+      <c r="D118" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>200</v>
+      </c>
+      <c r="B119">
+        <v>8</v>
+      </c>
+      <c r="C119" s="16">
+        <v>0</v>
+      </c>
+      <c r="D119" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>201</v>
+      </c>
+      <c r="B120">
+        <v>26</v>
+      </c>
+      <c r="C120" s="16">
+        <v>0</v>
+      </c>
+      <c r="D120" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>202</v>
+      </c>
+      <c r="B121">
+        <v>26</v>
+      </c>
+      <c r="C121" s="16">
+        <v>0</v>
+      </c>
+      <c r="D121" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>203</v>
+      </c>
+      <c r="B122">
+        <v>35</v>
+      </c>
+      <c r="C122" s="16">
+        <v>0</v>
+      </c>
+      <c r="D122" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>204</v>
+      </c>
+      <c r="B123">
+        <v>11</v>
+      </c>
+      <c r="C123" s="16">
+        <v>0</v>
+      </c>
+      <c r="D123" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>205</v>
+      </c>
+      <c r="B124">
+        <v>11</v>
+      </c>
+      <c r="C124" s="16">
+        <v>0</v>
+      </c>
+      <c r="D124" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>206</v>
+      </c>
+      <c r="B125">
+        <v>33</v>
+      </c>
+      <c r="C125" s="16">
+        <v>0</v>
+      </c>
+      <c r="D125" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
+        <v>207</v>
+      </c>
+      <c r="B126">
+        <v>9</v>
+      </c>
+      <c r="C126" s="16">
+        <v>0</v>
+      </c>
+      <c r="D126" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>208</v>
+      </c>
+      <c r="B127">
+        <v>9</v>
+      </c>
+      <c r="C127" s="16">
+        <v>0</v>
+      </c>
+      <c r="D127" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
+        <v>209</v>
+      </c>
+      <c r="B128">
+        <v>25</v>
+      </c>
+      <c r="C128" s="16">
+        <v>0</v>
+      </c>
+      <c r="D128" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>210</v>
+      </c>
+      <c r="B129">
+        <v>27</v>
+      </c>
+      <c r="C129" s="16">
+        <v>0</v>
+      </c>
+      <c r="D129" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>211</v>
+      </c>
+      <c r="B130">
+        <v>12</v>
+      </c>
+      <c r="C130" s="16">
+        <v>0</v>
+      </c>
+      <c r="D130" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
+        <v>212</v>
+      </c>
+      <c r="B131">
+        <v>12</v>
+      </c>
+      <c r="C131" s="16">
+        <v>0</v>
+      </c>
+      <c r="D131" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>213</v>
+      </c>
+      <c r="B132">
+        <v>22</v>
+      </c>
+      <c r="C132" s="16">
+        <v>0</v>
+      </c>
+      <c r="D132" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>214</v>
+      </c>
+      <c r="B133">
+        <v>36</v>
+      </c>
+      <c r="C133" s="16">
+        <v>0</v>
+      </c>
+      <c r="D133" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="s">
+        <v>215</v>
+      </c>
+      <c r="B134">
+        <v>22</v>
+      </c>
+      <c r="C134" s="16">
+        <v>0</v>
+      </c>
+      <c r="D134" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="s">
+        <v>216</v>
+      </c>
+      <c r="B135">
+        <v>30</v>
+      </c>
+      <c r="C135" s="16">
+        <v>0</v>
+      </c>
+      <c r="D135" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="s">
+        <v>217</v>
+      </c>
+      <c r="B136">
+        <v>30</v>
+      </c>
+      <c r="C136" s="16">
+        <v>0</v>
+      </c>
+      <c r="D136" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" t="s">
+        <v>218</v>
+      </c>
+      <c r="B137">
+        <v>29</v>
+      </c>
+      <c r="C137" s="16">
+        <v>0</v>
+      </c>
+      <c r="D137" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" t="s">
+        <v>219</v>
+      </c>
+      <c r="B138">
+        <v>20</v>
+      </c>
+      <c r="C138" s="16">
+        <v>0</v>
+      </c>
+      <c r="D138" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" t="s">
+        <v>220</v>
+      </c>
+      <c r="B139">
+        <v>20</v>
+      </c>
+      <c r="C139" s="16">
+        <v>0</v>
+      </c>
+      <c r="D139" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" t="s">
+        <v>221</v>
+      </c>
+      <c r="B140">
+        <v>32</v>
+      </c>
+      <c r="C140" s="16">
+        <v>0</v>
+      </c>
+      <c r="D140" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" t="s">
+        <v>222</v>
+      </c>
+      <c r="B141">
+        <v>28</v>
+      </c>
+      <c r="C141" s="16">
+        <v>0</v>
+      </c>
+      <c r="D141" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" t="s">
+        <v>223</v>
+      </c>
+      <c r="B142">
+        <v>12</v>
+      </c>
+      <c r="C142" s="16">
+        <v>0</v>
+      </c>
+      <c r="D142" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" t="s">
+        <v>224</v>
+      </c>
+      <c r="B143">
+        <v>28</v>
+      </c>
+      <c r="C143" s="16">
+        <v>0</v>
+      </c>
+      <c r="D143" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" t="s">
+        <v>225</v>
+      </c>
+      <c r="B144">
+        <v>13</v>
+      </c>
+      <c r="C144" s="16">
+        <v>0</v>
+      </c>
+      <c r="D144" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" t="s">
+        <v>226</v>
+      </c>
+      <c r="B145">
+        <v>14</v>
+      </c>
+      <c r="C145" s="16">
+        <v>0</v>
+      </c>
+      <c r="D145" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" t="s">
+        <v>227</v>
+      </c>
+      <c r="B146">
+        <v>13</v>
+      </c>
+      <c r="C146" s="16">
+        <v>0</v>
+      </c>
+      <c r="D146" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" t="s">
+        <v>228</v>
+      </c>
+      <c r="B147">
+        <v>38</v>
+      </c>
+      <c r="C147" s="16">
+        <v>0</v>
+      </c>
+      <c r="D147" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" t="s">
+        <v>229</v>
+      </c>
+      <c r="B148">
+        <v>34</v>
+      </c>
+      <c r="C148" s="16">
+        <v>0</v>
+      </c>
+      <c r="D148" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>230</v>
+      </c>
+      <c r="B149">
+        <v>38</v>
+      </c>
+      <c r="C149" s="16">
+        <v>0</v>
+      </c>
+      <c r="D149" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="s">
+        <v>231</v>
+      </c>
+      <c r="B150">
+        <v>38</v>
+      </c>
+      <c r="C150" s="16">
+        <v>0</v>
+      </c>
+      <c r="D150" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" t="s">
+        <v>232</v>
+      </c>
+      <c r="B151">
+        <v>34</v>
+      </c>
+      <c r="C151" s="16">
+        <v>0</v>
+      </c>
+      <c r="D151" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" t="s">
+        <v>233</v>
+      </c>
+      <c r="B152">
+        <v>31</v>
+      </c>
+      <c r="C152" s="16">
+        <v>0</v>
+      </c>
+      <c r="D152" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" t="s">
+        <v>234</v>
+      </c>
+      <c r="B153">
+        <v>39</v>
+      </c>
+      <c r="C153" s="16">
+        <v>0</v>
+      </c>
+      <c r="D153" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" t="s">
+        <v>235</v>
+      </c>
+      <c r="B154">
+        <v>31</v>
+      </c>
+      <c r="C154" s="16">
+        <v>0</v>
+      </c>
+      <c r="D154" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" t="s">
+        <v>236</v>
+      </c>
+      <c r="B155">
+        <v>31</v>
+      </c>
+      <c r="C155" s="16">
+        <v>0</v>
+      </c>
+      <c r="D155" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="s">
+        <v>237</v>
+      </c>
+      <c r="B156">
+        <v>15</v>
+      </c>
+      <c r="C156" s="16">
+        <v>0</v>
+      </c>
+      <c r="D156" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" t="s">
+        <v>238</v>
+      </c>
+      <c r="B157">
+        <v>14</v>
+      </c>
+      <c r="C157" s="16">
+        <v>0</v>
+      </c>
+      <c r="D157" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" t="s">
+        <v>239</v>
+      </c>
+      <c r="B158">
+        <v>14</v>
+      </c>
+      <c r="C158" s="16">
+        <v>0</v>
+      </c>
+      <c r="D158" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159">
+        <v>14</v>
+      </c>
+      <c r="B159" t="s">
+        <v>79</v>
+      </c>
+      <c r="C159" s="16">
+        <v>0</v>
+      </c>
+      <c r="D159" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160">
+        <v>12</v>
+      </c>
+      <c r="B160" t="s">
+        <v>81</v>
+      </c>
+      <c r="C160" s="16">
+        <v>0</v>
+      </c>
+      <c r="D160" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161">
+        <v>12</v>
+      </c>
+      <c r="B161" t="s">
+        <v>83</v>
+      </c>
+      <c r="C161" s="16">
+        <v>0</v>
+      </c>
+      <c r="D161" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162">
+        <v>15</v>
+      </c>
+      <c r="B162" t="s">
+        <v>84</v>
+      </c>
+      <c r="C162" s="16">
+        <v>0</v>
+      </c>
+      <c r="D162" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163">
+        <v>25</v>
+      </c>
+      <c r="B163" t="s">
+        <v>85</v>
+      </c>
+      <c r="C163" s="16">
+        <v>0</v>
+      </c>
+      <c r="D163" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164">
+        <v>24</v>
+      </c>
+      <c r="B164" t="s">
+        <v>86</v>
+      </c>
+      <c r="C164" s="16">
+        <v>0</v>
+      </c>
+      <c r="D164" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165">
+        <v>7</v>
+      </c>
+      <c r="B165" t="s">
+        <v>87</v>
+      </c>
+      <c r="C165" s="16">
+        <v>0</v>
+      </c>
+      <c r="D165" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166">
+        <v>8</v>
+      </c>
+      <c r="B166" t="s">
+        <v>89</v>
+      </c>
+      <c r="C166" s="16">
+        <v>0</v>
+      </c>
+      <c r="D166" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167">
+        <v>9</v>
+      </c>
+      <c r="B167" t="s">
+        <v>90</v>
+      </c>
+      <c r="C167" s="16">
+        <v>0</v>
+      </c>
+      <c r="D167" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168">
+        <v>10</v>
+      </c>
+      <c r="B168" t="s">
+        <v>91</v>
+      </c>
+      <c r="C168" s="16">
+        <v>0</v>
+      </c>
+      <c r="D168" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169">
+        <v>11</v>
+      </c>
+      <c r="B169" t="s">
+        <v>92</v>
+      </c>
+      <c r="C169" s="16">
+        <v>0</v>
+      </c>
+      <c r="D169" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170">
+        <v>12</v>
+      </c>
+      <c r="B170" t="s">
+        <v>93</v>
+      </c>
+      <c r="C170" s="16">
+        <v>0</v>
+      </c>
+      <c r="D170" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171">
+        <v>13</v>
+      </c>
+      <c r="B171" t="s">
+        <v>94</v>
+      </c>
+      <c r="C171" s="16">
+        <v>0</v>
+      </c>
+      <c r="D171" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172">
+        <v>14</v>
+      </c>
+      <c r="B172" t="s">
+        <v>95</v>
+      </c>
+      <c r="C172" s="16">
+        <v>0</v>
+      </c>
+      <c r="D172" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173">
+        <v>15</v>
+      </c>
+      <c r="B173" t="s">
+        <v>96</v>
+      </c>
+      <c r="C173" s="16">
+        <v>0</v>
+      </c>
+      <c r="D173" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174">
+        <v>16</v>
+      </c>
+      <c r="B174" t="s">
+        <v>97</v>
+      </c>
+      <c r="C174" s="16">
+        <v>0</v>
+      </c>
+      <c r="D174" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175">
+        <v>17</v>
+      </c>
+      <c r="B175" t="s">
+        <v>98</v>
+      </c>
+      <c r="C175" s="16">
+        <v>0</v>
+      </c>
+      <c r="D175" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176">
+        <v>18</v>
+      </c>
+      <c r="B176" t="s">
+        <v>99</v>
+      </c>
+      <c r="C176" s="16">
+        <v>0</v>
+      </c>
+      <c r="D176" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177">
+        <v>19</v>
+      </c>
+      <c r="B177" t="s">
+        <v>100</v>
+      </c>
+      <c r="C177" s="16">
+        <v>0</v>
+      </c>
+      <c r="D177" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178">
+        <v>20</v>
+      </c>
+      <c r="B178" t="s">
+        <v>101</v>
+      </c>
+      <c r="C178" s="16">
+        <v>0</v>
+      </c>
+      <c r="D178" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179">
+        <v>21</v>
+      </c>
+      <c r="B179" t="s">
+        <v>102</v>
+      </c>
+      <c r="C179" s="16">
+        <v>0</v>
+      </c>
+      <c r="D179" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180">
+        <v>22</v>
+      </c>
+      <c r="B180" t="s">
+        <v>103</v>
+      </c>
+      <c r="C180" s="16">
+        <v>0</v>
+      </c>
+      <c r="D180" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181">
+        <v>23</v>
+      </c>
+      <c r="B181" t="s">
+        <v>104</v>
+      </c>
+      <c r="C181" s="16">
+        <v>0</v>
+      </c>
+      <c r="D181" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182">
+        <v>24</v>
+      </c>
+      <c r="B182" t="s">
+        <v>105</v>
+      </c>
+      <c r="C182" s="16">
+        <v>0</v>
+      </c>
+      <c r="D182" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183">
+        <v>25</v>
+      </c>
+      <c r="B183" t="s">
+        <v>106</v>
+      </c>
+      <c r="C183" s="16">
+        <v>0</v>
+      </c>
+      <c r="D183" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184">
+        <v>26</v>
+      </c>
+      <c r="B184" t="s">
+        <v>107</v>
+      </c>
+      <c r="C184" s="16">
+        <v>0</v>
+      </c>
+      <c r="D184" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185">
+        <v>27</v>
+      </c>
+      <c r="B185" t="s">
+        <v>108</v>
+      </c>
+      <c r="C185" s="16">
+        <v>0</v>
+      </c>
+      <c r="D185" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186">
+        <v>28</v>
+      </c>
+      <c r="B186" t="s">
+        <v>109</v>
+      </c>
+      <c r="C186" s="16">
+        <v>0</v>
+      </c>
+      <c r="D186" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187">
+        <v>29</v>
+      </c>
+      <c r="B187" t="s">
+        <v>110</v>
+      </c>
+      <c r="C187" s="16">
+        <v>0</v>
+      </c>
+      <c r="D187" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188">
+        <v>30</v>
+      </c>
+      <c r="B188" t="s">
+        <v>111</v>
+      </c>
+      <c r="C188" s="16">
+        <v>0</v>
+      </c>
+      <c r="D188" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189">
+        <v>31</v>
+      </c>
+      <c r="B189" t="s">
+        <v>112</v>
+      </c>
+      <c r="C189" s="16">
+        <v>0</v>
+      </c>
+      <c r="D189" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190">
+        <v>32</v>
+      </c>
+      <c r="B190" t="s">
+        <v>113</v>
+      </c>
+      <c r="C190" s="16">
+        <v>0</v>
+      </c>
+      <c r="D190" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191">
+        <v>33</v>
+      </c>
+      <c r="B191" t="s">
+        <v>114</v>
+      </c>
+      <c r="C191" s="16">
+        <v>0</v>
+      </c>
+      <c r="D191" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192">
+        <v>34</v>
+      </c>
+      <c r="B192" t="s">
+        <v>115</v>
+      </c>
+      <c r="C192" s="16">
+        <v>0</v>
+      </c>
+      <c r="D192" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193">
+        <v>35</v>
+      </c>
+      <c r="B193" t="s">
+        <v>116</v>
+      </c>
+      <c r="C193" s="16">
+        <v>0</v>
+      </c>
+      <c r="D193" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194">
+        <v>36</v>
+      </c>
+      <c r="B194" t="s">
+        <v>117</v>
+      </c>
+      <c r="C194" s="16">
+        <v>0</v>
+      </c>
+      <c r="D194" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195">
+        <v>37</v>
+      </c>
+      <c r="B195" t="s">
+        <v>118</v>
+      </c>
+      <c r="C195" s="16">
+        <v>0</v>
+      </c>
+      <c r="D195" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196">
+        <v>38</v>
+      </c>
+      <c r="B196" t="s">
+        <v>119</v>
+      </c>
+      <c r="C196" s="16">
+        <v>0</v>
+      </c>
+      <c r="D196" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197">
+        <v>39</v>
+      </c>
+      <c r="B197" t="s">
+        <v>120</v>
+      </c>
+      <c r="C197" s="16">
+        <v>0</v>
+      </c>
+      <c r="D197" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198">
+        <v>25</v>
+      </c>
+      <c r="B198" t="s">
+        <v>121</v>
+      </c>
+      <c r="C198" s="16">
+        <v>0</v>
+      </c>
+      <c r="D198" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199">
+        <v>25</v>
+      </c>
+      <c r="B199" t="s">
+        <v>123</v>
+      </c>
+      <c r="C199" s="16">
+        <v>0</v>
+      </c>
+      <c r="D199" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200">
+        <v>24</v>
+      </c>
+      <c r="B200" t="s">
+        <v>124</v>
+      </c>
+      <c r="C200" s="16">
+        <v>0</v>
+      </c>
+      <c r="D200" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201">
+        <v>25</v>
+      </c>
+      <c r="B201" t="s">
+        <v>125</v>
+      </c>
+      <c r="C201" s="16">
+        <v>0</v>
+      </c>
+      <c r="D201" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202">
+        <v>24</v>
+      </c>
+      <c r="B202" t="s">
+        <v>126</v>
+      </c>
+      <c r="C202" s="16">
+        <v>0</v>
+      </c>
+      <c r="D202" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203">
+        <v>24</v>
+      </c>
+      <c r="B203" t="s">
+        <v>127</v>
+      </c>
+      <c r="C203" s="16">
+        <v>0</v>
+      </c>
+      <c r="D203" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204">
+        <v>24</v>
+      </c>
+      <c r="B204" t="s">
+        <v>128</v>
+      </c>
+      <c r="C204" s="16">
+        <v>0</v>
+      </c>
+      <c r="D204" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205">
+        <v>24</v>
+      </c>
+      <c r="B205" t="s">
+        <v>129</v>
+      </c>
+      <c r="C205" s="16">
+        <v>0</v>
+      </c>
+      <c r="D205" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206">
+        <v>24</v>
+      </c>
+      <c r="B206" t="s">
+        <v>130</v>
+      </c>
+      <c r="C206" s="16">
+        <v>0</v>
+      </c>
+      <c r="D206" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207">
+        <v>24</v>
+      </c>
+      <c r="B207" t="s">
+        <v>131</v>
+      </c>
+      <c r="C207" s="16">
+        <v>0</v>
+      </c>
+      <c r="D207" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208">
+        <v>25</v>
+      </c>
+      <c r="B208" t="s">
+        <v>132</v>
+      </c>
+      <c r="C208" s="16">
+        <v>0</v>
+      </c>
+      <c r="D208" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209">
+        <v>25</v>
+      </c>
+      <c r="B209" t="s">
+        <v>133</v>
+      </c>
+      <c r="C209" s="16">
+        <v>0</v>
+      </c>
+      <c r="D209" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210">
+        <v>24</v>
+      </c>
+      <c r="B210" t="s">
+        <v>134</v>
+      </c>
+      <c r="C210" s="16">
+        <v>0</v>
+      </c>
+      <c r="D210" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211">
+        <v>24</v>
+      </c>
+      <c r="B211" t="s">
+        <v>135</v>
+      </c>
+      <c r="C211" s="16">
+        <v>0</v>
+      </c>
+      <c r="D211" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212">
+        <v>25</v>
+      </c>
+      <c r="B212" t="s">
+        <v>136</v>
+      </c>
+      <c r="C212" s="16">
+        <v>0</v>
+      </c>
+      <c r="D212" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213">
+        <v>24</v>
+      </c>
+      <c r="B213" t="s">
+        <v>137</v>
+      </c>
+      <c r="C213" s="16">
+        <v>0</v>
+      </c>
+      <c r="D213" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214">
+        <v>24</v>
+      </c>
+      <c r="B214" t="s">
+        <v>138</v>
+      </c>
+      <c r="C214" s="16">
+        <v>0</v>
+      </c>
+      <c r="D214" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215">
+        <v>24</v>
+      </c>
+      <c r="B215" t="s">
+        <v>139</v>
+      </c>
+      <c r="C215" s="16">
+        <v>0</v>
+      </c>
+      <c r="D215" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216">
+        <v>10</v>
+      </c>
+      <c r="B216" t="s">
+        <v>140</v>
+      </c>
+      <c r="C216" s="16">
+        <v>0</v>
+      </c>
+      <c r="D216" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217">
+        <v>7</v>
+      </c>
+      <c r="B217" t="s">
+        <v>141</v>
+      </c>
+      <c r="C217" s="16">
+        <v>0</v>
+      </c>
+      <c r="D217" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218">
+        <v>7</v>
+      </c>
+      <c r="B218" t="s">
+        <v>142</v>
+      </c>
+      <c r="C218" s="16">
+        <v>0</v>
+      </c>
+      <c r="D218" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
+      <c r="A219">
+        <v>7</v>
+      </c>
+      <c r="B219" t="s">
+        <v>143</v>
+      </c>
+      <c r="C219" s="16">
+        <v>0</v>
+      </c>
+      <c r="D219" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4">
+      <c r="A220">
+        <v>10</v>
+      </c>
+      <c r="B220" t="s">
+        <v>144</v>
+      </c>
+      <c r="C220" s="16">
+        <v>0</v>
+      </c>
+      <c r="D220" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221">
+        <v>7</v>
+      </c>
+      <c r="B221" t="s">
+        <v>145</v>
+      </c>
+      <c r="C221" s="16">
+        <v>0</v>
+      </c>
+      <c r="D221" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222">
+        <v>10</v>
+      </c>
+      <c r="B222" t="s">
+        <v>146</v>
+      </c>
+      <c r="C222" s="16">
+        <v>0</v>
+      </c>
+      <c r="D222" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223">
+        <v>7</v>
+      </c>
+      <c r="B223" t="s">
+        <v>147</v>
+      </c>
+      <c r="C223" s="16">
+        <v>0</v>
+      </c>
+      <c r="D223" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224">
+        <v>7</v>
+      </c>
+      <c r="B224" t="s">
+        <v>148</v>
+      </c>
+      <c r="C224" s="16">
+        <v>0</v>
+      </c>
+      <c r="D224" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225">
+        <v>7</v>
+      </c>
+      <c r="B225" t="s">
+        <v>149</v>
+      </c>
+      <c r="C225" s="16">
+        <v>0</v>
+      </c>
+      <c r="D225" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4">
+      <c r="A226">
+        <v>10</v>
+      </c>
+      <c r="B226" t="s">
+        <v>150</v>
+      </c>
+      <c r="C226" s="16">
+        <v>0</v>
+      </c>
+      <c r="D226" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4">
+      <c r="A227">
+        <v>7</v>
+      </c>
+      <c r="B227" t="s">
+        <v>151</v>
+      </c>
+      <c r="C227" s="16">
+        <v>0</v>
+      </c>
+      <c r="D227" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4">
+      <c r="A228">
+        <v>10</v>
+      </c>
+      <c r="B228" t="s">
+        <v>152</v>
+      </c>
+      <c r="C228" s="16">
+        <v>0</v>
+      </c>
+      <c r="D228" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4">
+      <c r="A229">
+        <v>10</v>
+      </c>
+      <c r="B229" t="s">
+        <v>153</v>
+      </c>
+      <c r="C229" s="16">
+        <v>0</v>
+      </c>
+      <c r="D229" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4">
+      <c r="A230">
+        <v>10</v>
+      </c>
+      <c r="B230" t="s">
+        <v>154</v>
+      </c>
+      <c r="C230" s="16">
+        <v>0</v>
+      </c>
+      <c r="D230" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4">
+      <c r="A231">
+        <v>10</v>
+      </c>
+      <c r="B231" t="s">
+        <v>155</v>
+      </c>
+      <c r="C231" s="16">
+        <v>0</v>
+      </c>
+      <c r="D231" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4">
+      <c r="A232">
+        <v>10</v>
+      </c>
+      <c r="B232" t="s">
+        <v>156</v>
+      </c>
+      <c r="C232" s="16">
+        <v>0</v>
+      </c>
+      <c r="D232" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4">
+      <c r="A233">
+        <v>10</v>
+      </c>
+      <c r="B233" t="s">
+        <v>157</v>
+      </c>
+      <c r="C233" s="16">
+        <v>0</v>
+      </c>
+      <c r="D233" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4">
+      <c r="A234">
+        <v>37</v>
+      </c>
+      <c r="B234" t="s">
+        <v>158</v>
+      </c>
+      <c r="C234" s="16">
+        <v>0</v>
+      </c>
+      <c r="D234" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4">
+      <c r="A235">
+        <v>37</v>
+      </c>
+      <c r="B235" t="s">
+        <v>159</v>
+      </c>
+      <c r="C235" s="16">
+        <v>0</v>
+      </c>
+      <c r="D235" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4">
+      <c r="A236">
+        <v>37</v>
+      </c>
+      <c r="B236" t="s">
+        <v>160</v>
+      </c>
+      <c r="C236" s="16">
+        <v>0</v>
+      </c>
+      <c r="D236" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4">
+      <c r="A237">
+        <v>37</v>
+      </c>
+      <c r="B237" t="s">
+        <v>161</v>
+      </c>
+      <c r="C237" s="16">
+        <v>0</v>
+      </c>
+      <c r="D237" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4">
+      <c r="A238">
+        <v>37</v>
+      </c>
+      <c r="B238" t="s">
+        <v>162</v>
+      </c>
+      <c r="C238" s="16">
+        <v>0</v>
+      </c>
+      <c r="D238" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4">
+      <c r="A239">
+        <v>37</v>
+      </c>
+      <c r="B239" t="s">
+        <v>163</v>
+      </c>
+      <c r="C239" s="16">
+        <v>0</v>
+      </c>
+      <c r="D239" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4">
+      <c r="A240">
+        <v>37</v>
+      </c>
+      <c r="B240" t="s">
+        <v>164</v>
+      </c>
+      <c r="C240" s="16">
+        <v>0</v>
+      </c>
+      <c r="D240" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4">
+      <c r="A241">
+        <v>37</v>
+      </c>
+      <c r="B241" t="s">
+        <v>165</v>
+      </c>
+      <c r="C241" s="16">
+        <v>0</v>
+      </c>
+      <c r="D241" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4">
+      <c r="A242">
+        <v>37</v>
+      </c>
+      <c r="B242" t="s">
+        <v>166</v>
+      </c>
+      <c r="C242" s="16">
+        <v>0</v>
+      </c>
+      <c r="D242" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4">
+      <c r="A243">
+        <v>37</v>
+      </c>
+      <c r="B243" t="s">
+        <v>167</v>
+      </c>
+      <c r="C243" s="16">
+        <v>0</v>
+      </c>
+      <c r="D243" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4">
+      <c r="A244">
+        <v>37</v>
+      </c>
+      <c r="B244" t="s">
+        <v>168</v>
+      </c>
+      <c r="C244" s="16">
+        <v>0</v>
+      </c>
+      <c r="D244" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4">
+      <c r="A245">
+        <v>39</v>
+      </c>
+      <c r="B245" t="s">
+        <v>169</v>
+      </c>
+      <c r="C245" s="16">
+        <v>0</v>
+      </c>
+      <c r="D245" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4">
+      <c r="A246">
+        <v>37</v>
+      </c>
+      <c r="B246" t="s">
+        <v>170</v>
+      </c>
+      <c r="C246" s="16">
+        <v>0</v>
+      </c>
+      <c r="D246" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4">
+      <c r="A247">
+        <v>39</v>
+      </c>
+      <c r="B247" t="s">
+        <v>171</v>
+      </c>
+      <c r="C247" s="16">
+        <v>0</v>
+      </c>
+      <c r="D247" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4">
+      <c r="A248">
+        <v>39</v>
+      </c>
+      <c r="B248" t="s">
+        <v>172</v>
+      </c>
+      <c r="C248" s="16">
+        <v>0</v>
+      </c>
+      <c r="D248" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4">
+      <c r="A249">
+        <v>39</v>
+      </c>
+      <c r="B249" t="s">
+        <v>173</v>
+      </c>
+      <c r="C249" s="16">
+        <v>0</v>
+      </c>
+      <c r="D249" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4">
+      <c r="A250">
+        <v>39</v>
+      </c>
+      <c r="B250" t="s">
+        <v>174</v>
+      </c>
+      <c r="C250" s="16">
+        <v>0</v>
+      </c>
+      <c r="D250" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4">
+      <c r="A251">
+        <v>37</v>
+      </c>
+      <c r="B251" t="s">
+        <v>175</v>
+      </c>
+      <c r="C251" s="16">
+        <v>0</v>
+      </c>
+      <c r="D251" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4">
+      <c r="A252">
+        <v>19</v>
+      </c>
+      <c r="B252" t="s">
+        <v>176</v>
+      </c>
+      <c r="C252" s="16">
+        <v>0</v>
+      </c>
+      <c r="D252" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4">
+      <c r="A253">
+        <v>24</v>
+      </c>
+      <c r="B253" t="s">
+        <v>177</v>
+      </c>
+      <c r="C253" s="16">
+        <v>0</v>
+      </c>
+      <c r="D253" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4">
+      <c r="A254">
+        <v>15</v>
+      </c>
+      <c r="B254" t="s">
+        <v>178</v>
+      </c>
+      <c r="C254" s="16">
+        <v>0</v>
+      </c>
+      <c r="D254" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4">
+      <c r="A255">
+        <v>24</v>
+      </c>
+      <c r="B255" t="s">
+        <v>179</v>
+      </c>
+      <c r="C255" s="16">
+        <v>0</v>
+      </c>
+      <c r="D255" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4">
+      <c r="A256">
+        <v>15</v>
+      </c>
+      <c r="B256" t="s">
+        <v>180</v>
+      </c>
+      <c r="C256" s="16">
+        <v>0</v>
+      </c>
+      <c r="D256" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
+      <c r="A257">
+        <v>19</v>
+      </c>
+      <c r="B257" t="s">
+        <v>181</v>
+      </c>
+      <c r="C257" s="16">
+        <v>0</v>
+      </c>
+      <c r="D257" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
+      <c r="A258">
+        <v>15</v>
+      </c>
+      <c r="B258" t="s">
+        <v>182</v>
+      </c>
+      <c r="C258" s="16">
+        <v>0</v>
+      </c>
+      <c r="D258" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
+      <c r="A259">
+        <v>15</v>
+      </c>
+      <c r="B259" t="s">
+        <v>183</v>
+      </c>
+      <c r="C259" s="16">
+        <v>0</v>
+      </c>
+      <c r="D259" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4">
+      <c r="A260">
+        <v>19</v>
+      </c>
+      <c r="B260" t="s">
+        <v>184</v>
+      </c>
+      <c r="C260" s="16">
+        <v>0</v>
+      </c>
+      <c r="D260" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4">
+      <c r="A261">
+        <v>15</v>
+      </c>
+      <c r="B261" t="s">
+        <v>185</v>
+      </c>
+      <c r="C261" s="16">
+        <v>0</v>
+      </c>
+      <c r="D261" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4">
+      <c r="A262">
+        <v>16</v>
+      </c>
+      <c r="B262" t="s">
+        <v>186</v>
+      </c>
+      <c r="C262" s="16">
+        <v>0</v>
+      </c>
+      <c r="D262" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4">
+      <c r="A263">
+        <v>21</v>
+      </c>
+      <c r="B263" t="s">
+        <v>187</v>
+      </c>
+      <c r="C263" s="16">
+        <v>0</v>
+      </c>
+      <c r="D263" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4">
+      <c r="A264">
+        <v>16</v>
+      </c>
+      <c r="B264" t="s">
+        <v>188</v>
+      </c>
+      <c r="C264" s="16">
+        <v>0</v>
+      </c>
+      <c r="D264" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4">
+      <c r="A265">
+        <v>17</v>
+      </c>
+      <c r="B265" t="s">
+        <v>189</v>
+      </c>
+      <c r="C265" s="16">
+        <v>0</v>
+      </c>
+      <c r="D265" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4">
+      <c r="A266">
+        <v>23</v>
+      </c>
+      <c r="B266" t="s">
+        <v>190</v>
+      </c>
+      <c r="C266" s="16">
+        <v>0</v>
+      </c>
+      <c r="D266" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4">
+      <c r="A267">
+        <v>17</v>
+      </c>
+      <c r="B267" t="s">
+        <v>191</v>
+      </c>
+      <c r="C267" s="16">
+        <v>0</v>
+      </c>
+      <c r="D267" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4">
+      <c r="A268">
+        <v>18</v>
+      </c>
+      <c r="B268" t="s">
+        <v>192</v>
+      </c>
+      <c r="C268" s="16">
+        <v>0</v>
+      </c>
+      <c r="D268" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4">
+      <c r="A269">
+        <v>12</v>
+      </c>
+      <c r="B269" t="s">
+        <v>193</v>
+      </c>
+      <c r="C269" s="16">
+        <v>0</v>
+      </c>
+      <c r="D269" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4">
+      <c r="A270">
+        <v>18</v>
+      </c>
+      <c r="B270" t="s">
+        <v>194</v>
+      </c>
+      <c r="C270" s="16">
+        <v>0</v>
+      </c>
+      <c r="D270" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4">
+      <c r="A271">
+        <v>12</v>
+      </c>
+      <c r="B271" t="s">
+        <v>195</v>
+      </c>
+      <c r="C271" s="16">
+        <v>0</v>
+      </c>
+      <c r="D271" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4">
+      <c r="A272">
+        <v>12</v>
+      </c>
+      <c r="B272" t="s">
+        <v>196</v>
+      </c>
+      <c r="C272" s="16">
+        <v>0</v>
+      </c>
+      <c r="D272" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4">
+      <c r="A273">
+        <v>18</v>
+      </c>
+      <c r="B273" t="s">
+        <v>197</v>
+      </c>
+      <c r="C273" s="16">
+        <v>0</v>
+      </c>
+      <c r="D273" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4">
+      <c r="A274">
+        <v>11</v>
+      </c>
+      <c r="B274" t="s">
+        <v>198</v>
+      </c>
+      <c r="C274" s="16">
+        <v>0</v>
+      </c>
+      <c r="D274" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4">
+      <c r="A275">
+        <v>8</v>
+      </c>
+      <c r="B275" t="s">
+        <v>199</v>
+      </c>
+      <c r="C275" s="16">
+        <v>0</v>
+      </c>
+      <c r="D275" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4">
+      <c r="A276">
+        <v>8</v>
+      </c>
+      <c r="B276" t="s">
+        <v>200</v>
+      </c>
+      <c r="C276" s="16">
+        <v>0</v>
+      </c>
+      <c r="D276" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4">
+      <c r="A277">
+        <v>26</v>
+      </c>
+      <c r="B277" t="s">
+        <v>201</v>
+      </c>
+      <c r="C277" s="16">
+        <v>0</v>
+      </c>
+      <c r="D277" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4">
+      <c r="A278">
+        <v>26</v>
+      </c>
+      <c r="B278" t="s">
+        <v>202</v>
+      </c>
+      <c r="C278" s="16">
+        <v>0</v>
+      </c>
+      <c r="D278" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4">
+      <c r="A279">
+        <v>35</v>
+      </c>
+      <c r="B279" t="s">
+        <v>203</v>
+      </c>
+      <c r="C279" s="16">
+        <v>0</v>
+      </c>
+      <c r="D279" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4">
+      <c r="A280">
+        <v>11</v>
+      </c>
+      <c r="B280" t="s">
+        <v>204</v>
+      </c>
+      <c r="C280" s="16">
+        <v>0</v>
+      </c>
+      <c r="D280" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4">
+      <c r="A281">
+        <v>11</v>
+      </c>
+      <c r="B281" t="s">
+        <v>205</v>
+      </c>
+      <c r="C281" s="16">
+        <v>0</v>
+      </c>
+      <c r="D281" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4">
+      <c r="A282">
+        <v>33</v>
+      </c>
+      <c r="B282" t="s">
+        <v>206</v>
+      </c>
+      <c r="C282" s="16">
+        <v>0</v>
+      </c>
+      <c r="D282" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4">
+      <c r="A283">
+        <v>9</v>
+      </c>
+      <c r="B283" t="s">
+        <v>207</v>
+      </c>
+      <c r="C283" s="16">
+        <v>0</v>
+      </c>
+      <c r="D283" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4">
+      <c r="A284">
+        <v>9</v>
+      </c>
+      <c r="B284" t="s">
+        <v>208</v>
+      </c>
+      <c r="C284" s="16">
+        <v>0</v>
+      </c>
+      <c r="D284" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4">
+      <c r="A285">
+        <v>25</v>
+      </c>
+      <c r="B285" t="s">
+        <v>209</v>
+      </c>
+      <c r="C285" s="16">
+        <v>0</v>
+      </c>
+      <c r="D285" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4">
+      <c r="A286">
+        <v>27</v>
+      </c>
+      <c r="B286" t="s">
+        <v>210</v>
+      </c>
+      <c r="C286" s="16">
+        <v>0</v>
+      </c>
+      <c r="D286" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4">
+      <c r="A287">
+        <v>12</v>
+      </c>
+      <c r="B287" t="s">
+        <v>211</v>
+      </c>
+      <c r="C287" s="16">
+        <v>0</v>
+      </c>
+      <c r="D287" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4">
+      <c r="A288">
+        <v>12</v>
+      </c>
+      <c r="B288" t="s">
+        <v>212</v>
+      </c>
+      <c r="C288" s="16">
+        <v>0</v>
+      </c>
+      <c r="D288" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4">
+      <c r="A289">
+        <v>22</v>
+      </c>
+      <c r="B289" t="s">
+        <v>213</v>
+      </c>
+      <c r="C289" s="16">
+        <v>0</v>
+      </c>
+      <c r="D289" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4">
+      <c r="A290">
+        <v>36</v>
+      </c>
+      <c r="B290" t="s">
+        <v>214</v>
+      </c>
+      <c r="C290" s="16">
+        <v>0</v>
+      </c>
+      <c r="D290" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4">
+      <c r="A291">
+        <v>22</v>
+      </c>
+      <c r="B291" t="s">
+        <v>215</v>
+      </c>
+      <c r="C291" s="16">
+        <v>0</v>
+      </c>
+      <c r="D291" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4">
+      <c r="A292">
+        <v>30</v>
+      </c>
+      <c r="B292" t="s">
+        <v>216</v>
+      </c>
+      <c r="C292" s="16">
+        <v>0</v>
+      </c>
+      <c r="D292" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4">
+      <c r="A293">
+        <v>30</v>
+      </c>
+      <c r="B293" t="s">
+        <v>217</v>
+      </c>
+      <c r="C293" s="16">
+        <v>0</v>
+      </c>
+      <c r="D293" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4">
+      <c r="A294">
+        <v>29</v>
+      </c>
+      <c r="B294" t="s">
+        <v>218</v>
+      </c>
+      <c r="C294" s="16">
+        <v>0</v>
+      </c>
+      <c r="D294" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4">
+      <c r="A295">
+        <v>20</v>
+      </c>
+      <c r="B295" t="s">
+        <v>219</v>
+      </c>
+      <c r="C295" s="16">
+        <v>0</v>
+      </c>
+      <c r="D295" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4">
+      <c r="A296">
+        <v>20</v>
+      </c>
+      <c r="B296" t="s">
+        <v>220</v>
+      </c>
+      <c r="C296" s="16">
+        <v>0</v>
+      </c>
+      <c r="D296" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4">
+      <c r="A297">
+        <v>32</v>
+      </c>
+      <c r="B297" t="s">
+        <v>221</v>
+      </c>
+      <c r="C297" s="16">
+        <v>0</v>
+      </c>
+      <c r="D297" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4">
+      <c r="A298">
+        <v>28</v>
+      </c>
+      <c r="B298" t="s">
+        <v>222</v>
+      </c>
+      <c r="C298" s="16">
+        <v>0</v>
+      </c>
+      <c r="D298" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4">
+      <c r="A299">
+        <v>12</v>
+      </c>
+      <c r="B299" t="s">
+        <v>223</v>
+      </c>
+      <c r="C299" s="16">
+        <v>0</v>
+      </c>
+      <c r="D299" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4">
+      <c r="A300">
+        <v>28</v>
+      </c>
+      <c r="B300" t="s">
+        <v>224</v>
+      </c>
+      <c r="C300" s="16">
+        <v>0</v>
+      </c>
+      <c r="D300" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4">
+      <c r="A301">
+        <v>13</v>
+      </c>
+      <c r="B301" t="s">
+        <v>225</v>
+      </c>
+      <c r="C301" s="16">
+        <v>0</v>
+      </c>
+      <c r="D301" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4">
+      <c r="A302">
+        <v>14</v>
+      </c>
+      <c r="B302" t="s">
+        <v>226</v>
+      </c>
+      <c r="C302" s="16">
+        <v>0</v>
+      </c>
+      <c r="D302" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4">
+      <c r="A303">
+        <v>13</v>
+      </c>
+      <c r="B303" t="s">
+        <v>227</v>
+      </c>
+      <c r="C303" s="16">
+        <v>0</v>
+      </c>
+      <c r="D303" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4">
+      <c r="A304">
+        <v>38</v>
+      </c>
+      <c r="B304" t="s">
+        <v>228</v>
+      </c>
+      <c r="C304" s="16">
+        <v>0</v>
+      </c>
+      <c r="D304" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4">
+      <c r="A305">
+        <v>34</v>
+      </c>
+      <c r="B305" t="s">
+        <v>229</v>
+      </c>
+      <c r="C305" s="16">
+        <v>0</v>
+      </c>
+      <c r="D305" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4">
+      <c r="A306">
+        <v>38</v>
+      </c>
+      <c r="B306" t="s">
+        <v>230</v>
+      </c>
+      <c r="C306" s="16">
+        <v>0</v>
+      </c>
+      <c r="D306" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4">
+      <c r="A307">
+        <v>38</v>
+      </c>
+      <c r="B307" t="s">
+        <v>231</v>
+      </c>
+      <c r="C307" s="16">
+        <v>0</v>
+      </c>
+      <c r="D307" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4">
+      <c r="A308">
+        <v>34</v>
+      </c>
+      <c r="B308" t="s">
+        <v>232</v>
+      </c>
+      <c r="C308" s="16">
+        <v>0</v>
+      </c>
+      <c r="D308" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4">
+      <c r="A309">
+        <v>31</v>
+      </c>
+      <c r="B309" t="s">
+        <v>233</v>
+      </c>
+      <c r="C309" s="16">
+        <v>0</v>
+      </c>
+      <c r="D309" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4">
+      <c r="A310">
+        <v>39</v>
+      </c>
+      <c r="B310" t="s">
+        <v>234</v>
+      </c>
+      <c r="C310" s="16">
+        <v>0</v>
+      </c>
+      <c r="D310" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4">
+      <c r="A311">
+        <v>31</v>
+      </c>
+      <c r="B311" t="s">
+        <v>235</v>
+      </c>
+      <c r="C311" s="16">
+        <v>0</v>
+      </c>
+      <c r="D311" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4">
+      <c r="A312">
+        <v>31</v>
+      </c>
+      <c r="B312" t="s">
+        <v>236</v>
+      </c>
+      <c r="C312" s="16">
+        <v>0</v>
+      </c>
+      <c r="D312" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4">
+      <c r="A313">
+        <v>15</v>
+      </c>
+      <c r="B313" t="s">
+        <v>237</v>
+      </c>
+      <c r="C313" s="16">
+        <v>0</v>
+      </c>
+      <c r="D313" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4">
+      <c r="A314">
+        <v>14</v>
+      </c>
+      <c r="B314" t="s">
+        <v>238</v>
+      </c>
+      <c r="C314" s="16">
+        <v>0</v>
+      </c>
+      <c r="D314" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4">
+      <c r="A315">
+        <v>14</v>
+      </c>
+      <c r="B315" t="s">
+        <v>239</v>
+      </c>
+      <c r="C315" s="16">
+        <v>0</v>
+      </c>
+      <c r="D315" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4">
+      <c r="D316" s="16"/>
+    </row>
+    <row r="317" spans="1:4">
+      <c r="D317" s="16"/>
+    </row>
+    <row r="318" spans="1:4">
+      <c r="D318" s="16"/>
+    </row>
+    <row r="319" spans="1:4">
+      <c r="D319" s="16"/>
+    </row>
+    <row r="320" spans="1:4">
+      <c r="D320" s="16"/>
+    </row>
+    <row r="321" spans="4:4">
+      <c r="D321" s="16"/>
+    </row>
+    <row r="322" spans="4:4">
+      <c r="D322" s="16"/>
+    </row>
+    <row r="323" spans="4:4">
+      <c r="D323" s="16"/>
+    </row>
+    <row r="324" spans="4:4">
+      <c r="D324" s="16"/>
+    </row>
+    <row r="325" spans="4:4">
+      <c r="D325" s="16"/>
+    </row>
+    <row r="326" spans="4:4">
+      <c r="D326" s="16"/>
+    </row>
+    <row r="327" spans="4:4">
+      <c r="D327" s="16"/>
+    </row>
+    <row r="328" spans="4:4">
+      <c r="D328" s="16"/>
+    </row>
+    <row r="329" spans="4:4">
+      <c r="D329" s="16"/>
+    </row>
+    <row r="330" spans="4:4">
+      <c r="D330" s="16"/>
+    </row>
+    <row r="331" spans="4:4">
+      <c r="D331" s="16"/>
+    </row>
+    <row r="332" spans="4:4">
+      <c r="D332" s="16"/>
+    </row>
+    <row r="333" spans="4:4">
+      <c r="D333" s="16"/>
+    </row>
+    <row r="334" spans="4:4">
+      <c r="D334" s="16"/>
+    </row>
+    <row r="335" spans="4:4">
+      <c r="D335" s="16"/>
+    </row>
+    <row r="336" spans="4:4">
+      <c r="D336" s="16"/>
+    </row>
+    <row r="337" spans="4:4">
+      <c r="D337" s="16"/>
+    </row>
+    <row r="338" spans="4:4">
+      <c r="D338" s="16"/>
+    </row>
+    <row r="339" spans="4:4">
+      <c r="D339" s="16"/>
+    </row>
+    <row r="340" spans="4:4">
+      <c r="D340" s="16"/>
+    </row>
+    <row r="341" spans="4:4">
+      <c r="D341" s="16"/>
+    </row>
+    <row r="342" spans="4:4">
+      <c r="D342" s="16"/>
+    </row>
+    <row r="343" spans="4:4">
+      <c r="D343" s="16"/>
+    </row>
+    <row r="344" spans="4:4">
+      <c r="D344" s="16"/>
+    </row>
+    <row r="345" spans="4:4">
+      <c r="D345" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA107B5-4444-3E49-88A6-FC27444C84E1}">
   <dimension ref="A1:D1802"/>
   <sheetViews>
@@ -17487,7 +22027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F250E95D-36D8-F94C-8819-AC12C7F47D5E}">
   <dimension ref="A1:E33"/>
   <sheetViews>
@@ -18124,7 +22664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2E83E6-EC55-124D-8909-8C3A7F43F28A}">
   <dimension ref="A1:C21"/>
   <sheetViews>

</xml_diff>